<commit_message>
Se mejoro la estructura del build DB
</commit_message>
<xml_diff>
--- a/proyecto_final_programacion_copia/src/main/java/co/edu/uniquindio/poo/Balance/Excel/Eventos_Personas.xlsx
+++ b/proyecto_final_programacion_copia/src/main/java/co/edu/uniquindio/poo/Balance/Excel/Eventos_Personas.xlsx
@@ -7,11 +7,10 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Shakira" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Kiss" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Kiss" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Colombia-Argentina" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Akash" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Colombia-Argentina" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="One Republic" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="One Direction" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -174,7 +173,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:t>Ingresos Comparativos por Tipo de Silla - Shakira</a:t>
+              <a:t>Ingresos Comparativos por Tipo de Silla - Kiss</a:t>
             </a:r>
           </a:p>
         </rich>
@@ -190,7 +189,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Shakira'!B12</f>
+              <f>'Kiss'!B9</f>
             </strRef>
           </tx>
           <spPr>
@@ -200,12 +199,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Shakira'!$A$13:$A$14</f>
+              <f>'Kiss'!$A$10:$A$11</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Shakira'!$B$13:$B$14</f>
+              <f>'Kiss'!$B$10:$B$11</f>
             </numRef>
           </val>
         </ser>
@@ -288,7 +287,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:t>Ingresos Comparativos por Tipo de Silla - Kiss</a:t>
+              <a:t>Ingresos Comparativos por Tipo de Silla - Colombia-Argentina</a:t>
             </a:r>
           </a:p>
         </rich>
@@ -304,7 +303,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Kiss'!B9</f>
+              <f>'Colombia-Argentina'!B9</f>
             </strRef>
           </tx>
           <spPr>
@@ -314,12 +313,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Kiss'!$A$10:$A$11</f>
+              <f>'Colombia-Argentina'!$A$10:$A$11</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Kiss'!$B$10:$B$11</f>
+              <f>'Colombia-Argentina'!$B$10:$B$11</f>
             </numRef>
           </val>
         </ser>
@@ -516,7 +515,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:t>Ingresos Comparativos por Tipo de Silla - Colombia-Argentina</a:t>
+              <a:t>Ingresos Comparativos por Tipo de Silla - One Direction</a:t>
             </a:r>
           </a:p>
         </rich>
@@ -532,7 +531,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Colombia-Argentina'!B8</f>
+              <f>'One Direction'!B10</f>
             </strRef>
           </tx>
           <spPr>
@@ -542,126 +541,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Colombia-Argentina'!$A$9:$A$10</f>
+              <f>'One Direction'!$A$11:$A$12</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Colombia-Argentina'!$B$9:$B$10</f>
-            </numRef>
-          </val>
-        </ser>
-        <gapWidth val="150"/>
-        <axId val="10"/>
-        <axId val="100"/>
-      </barChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Tipo de Silla</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Ingresos Totales</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="10"/>
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Ingresos Comparativos por Tipo de Silla - One Republic</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <barChart>
-        <barDir val="col"/>
-        <grouping val="clustered"/>
-        <varyColors val="1"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <strRef>
-              <f>'One Republic'!B9</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'One Republic'!$A$10:$A$11</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'One Republic'!$B$10:$B$11</f>
+              <f>'One Direction'!$B$11:$B$12</f>
             </numRef>
           </val>
         </ser>
@@ -737,7 +622,7 @@
     <from>
       <col>4</col>
       <colOff>0</colOff>
-      <row>11</row>
+      <row>8</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="5400000" cy="2700000"/>
@@ -818,34 +703,7 @@
     <from>
       <col>4</col>
       <colOff>0</colOff>
-      <row>7</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="1" name="Chart 1"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>4</col>
-      <colOff>0</colOff>
-      <row>8</row>
+      <row>9</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="5400000" cy="2700000"/>
@@ -1155,7 +1013,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1163,7 +1021,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="27" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
     <col width="10" customWidth="1" min="3" max="3"/>
     <col width="9" customWidth="1" min="4" max="4"/>
@@ -1174,7 +1032,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Detalles del Evento: Shakira</t>
+          <t>Detalles del Evento: Kiss</t>
         </is>
       </c>
     </row>
@@ -1213,11 +1071,11 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
-        <v>1234</v>
+        <v>1092455543</v>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>Carlos</t>
+          <t>Manuel</t>
         </is>
       </c>
       <c r="C4" s="3" t="n">
@@ -1232,16 +1090,16 @@
         </is>
       </c>
       <c r="F4" s="3" t="n">
-        <v>62500</v>
+        <v>312500</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
-        <v>1452</v>
+        <v>1094891731</v>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>manuel</t>
+          <t>Laura</t>
         </is>
       </c>
       <c r="C5" s="3" t="n">
@@ -1256,23 +1114,23 @@
         </is>
       </c>
       <c r="F5" s="3" t="n">
-        <v>62500</v>
+        <v>312500</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="n">
-        <v>23</v>
+        <v>1092455585</v>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>sadf</t>
+          <t>Leonardo</t>
         </is>
       </c>
       <c r="C6" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
@@ -1280,111 +1138,39 @@
         </is>
       </c>
       <c r="F6" s="3" t="n">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="n">
-        <v>134</v>
-      </c>
-      <c r="B7" s="3" t="inlineStr">
-        <is>
-          <t>wer</t>
-        </is>
-      </c>
-      <c r="C7" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="E7" s="3" t="inlineStr">
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="inlineStr">
+        <is>
+          <t>Tipo de Silla</t>
+        </is>
+      </c>
+      <c r="B9" s="4" t="inlineStr">
+        <is>
+          <t>Total Recaudado</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
         <is>
           <t>sillas_regular</t>
         </is>
       </c>
-      <c r="F7" s="3" t="n">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="n">
-        <v>44444</v>
-      </c>
-      <c r="B8" s="3" t="inlineStr">
-        <is>
-          <t>qwer</t>
-        </is>
-      </c>
-      <c r="C8" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="E8" s="3" t="inlineStr">
-        <is>
-          <t>sillas_regular</t>
-        </is>
-      </c>
-      <c r="F8" s="3" t="n">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="3" t="n">
-        <v>334</v>
-      </c>
-      <c r="B9" s="3" t="inlineStr">
-        <is>
-          <t>qwer</t>
-        </is>
-      </c>
-      <c r="C9" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E9" s="3" t="inlineStr">
-        <is>
-          <t>sillas_regular</t>
-        </is>
-      </c>
-      <c r="F9" s="3" t="n">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="4" t="inlineStr">
-        <is>
-          <t>Tipo de Silla</t>
-        </is>
-      </c>
-      <c r="B12" s="4" t="inlineStr">
-        <is>
-          <t>Total Recaudado</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>sillas_regular</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>200000</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="B10" t="n">
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
         <is>
           <t>sillas_vip</t>
         </is>
       </c>
-      <c r="B14" t="n">
-        <v>125000</v>
+      <c r="B11" t="n">
+        <v>625000</v>
       </c>
     </row>
   </sheetData>
@@ -1410,7 +1196,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="27" customWidth="1" min="1" max="1"/>
+    <col width="41" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
     <col width="10" customWidth="1" min="3" max="3"/>
     <col width="9" customWidth="1" min="4" max="4"/>
@@ -1421,7 +1207,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Detalles del Evento: Kiss</t>
+          <t>Detalles del Evento: Colombia-Argentina</t>
         </is>
       </c>
     </row>
@@ -1460,42 +1246,42 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
-        <v>14</v>
+        <v>1094895528</v>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>manuel</t>
+          <t>Santiago</t>
         </is>
       </c>
       <c r="C4" s="3" t="n">
         <v>2</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>sillas_regular</t>
+          <t>sillas_vip</t>
         </is>
       </c>
       <c r="F4" s="3" t="n">
-        <v>25000</v>
+        <v>300000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
-        <v>32</v>
+        <v>89489489</v>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>santiago</t>
+          <t>Leonardo</t>
         </is>
       </c>
       <c r="C5" s="3" t="n">
         <v>2</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
@@ -1503,31 +1289,31 @@
         </is>
       </c>
       <c r="F5" s="3" t="n">
-        <v>47500</v>
+        <v>300000</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="n">
-        <v>2323</v>
+        <v>1092455543</v>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>asdfsa</t>
+          <t>Manuel</t>
         </is>
       </c>
       <c r="C6" s="3" t="n">
         <v>2</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>sillas_vip</t>
+          <t>sillas_regular</t>
         </is>
       </c>
       <c r="F6" s="3" t="n">
-        <v>47500</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="9">
@@ -1549,7 +1335,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>25000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="11">
@@ -1559,7 +1345,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>95000</v>
+        <v>600000</v>
       </c>
     </row>
   </sheetData>
@@ -1635,11 +1421,11 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
-        <v>15</v>
+        <v>1092455543</v>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>manuel</t>
+          <t>Manuel</t>
         </is>
       </c>
       <c r="C4" s="3" t="n">
@@ -1654,47 +1440,47 @@
         </is>
       </c>
       <c r="F4" s="3" t="n">
-        <v>62500</v>
+        <v>55000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
-        <v>3232</v>
+        <v>1094891731</v>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>wqer</t>
+          <t>Laura</t>
         </is>
       </c>
       <c r="C5" s="3" t="n">
         <v>3</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>sillas_regular</t>
+          <t>sillas_vip</t>
         </is>
       </c>
       <c r="F5" s="3" t="n">
-        <v>50000</v>
+        <v>55000</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="n">
-        <v>1234</v>
+        <v>89005408</v>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>qwre</t>
+          <t>Ruben</t>
         </is>
       </c>
       <c r="C6" s="3" t="n">
         <v>3</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
@@ -1724,7 +1510,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>100000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="11">
@@ -1734,7 +1520,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>62500</v>
+        <v>110000</v>
       </c>
     </row>
   </sheetData>
@@ -1752,7 +1538,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1760,7 +1546,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="41" customWidth="1" min="1" max="1"/>
+    <col width="36" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
     <col width="10" customWidth="1" min="3" max="3"/>
     <col width="9" customWidth="1" min="4" max="4"/>
@@ -1771,7 +1557,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Detalles del Evento: Colombia-Argentina</t>
+          <t>Detalles del Evento: One Direction</t>
         </is>
       </c>
     </row>
@@ -1810,7 +1596,7 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
-        <v>1234</v>
+        <v>6526965</v>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
@@ -1829,182 +1615,31 @@
         </is>
       </c>
       <c r="F4" s="3" t="n">
-        <v>75000</v>
+        <v>195000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
-        <v>156198</v>
+        <v>6525695</v>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>Manuel</t>
+          <t>valentina</t>
         </is>
       </c>
       <c r="C5" s="3" t="n">
         <v>4</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>sillas_regular</t>
+          <t>sillas_vip</t>
         </is>
       </c>
       <c r="F5" s="3" t="n">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="inlineStr">
-        <is>
-          <t>Tipo de Silla</t>
-        </is>
-      </c>
-      <c r="B8" s="4" t="inlineStr">
-        <is>
-          <t>Total Recaudado</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>sillas_regular</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>sillas_vip</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>75000</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="35" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="10" customWidth="1" min="3" max="3"/>
-    <col width="9" customWidth="1" min="4" max="4"/>
-    <col width="16" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Detalles del Evento: One Republic</t>
-        </is>
-      </c>
-    </row>
-    <row r="2"/>
-    <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>idPersona</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>nombrePersona</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>idEvento</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
-          <t>idSilla</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="inlineStr">
-        <is>
-          <t>tipoSilla</t>
-        </is>
-      </c>
-      <c r="F3" s="2" t="inlineStr">
-        <is>
-          <t>totalPagar</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="n">
-        <v>828</v>
-      </c>
-      <c r="B4" s="3" t="inlineStr">
-        <is>
-          <t>DoÃ±a</t>
-        </is>
-      </c>
-      <c r="C4" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="D4" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="E4" s="3" t="inlineStr">
-        <is>
-          <t>sillas_vip</t>
-        </is>
-      </c>
-      <c r="F4" s="3" t="n">
-        <v>125000</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="n">
-        <v>1234</v>
-      </c>
-      <c r="B5" s="3" t="inlineStr">
-        <is>
-          <t>Carlos</t>
-        </is>
-      </c>
-      <c r="C5" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="D5" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E5" s="3" t="inlineStr">
-        <is>
-          <t>sillas_vip</t>
-        </is>
-      </c>
-      <c r="F5" s="3" t="n">
-        <v>125000</v>
+        <v>195000</v>
       </c>
     </row>
     <row r="6">
@@ -2017,50 +1652,74 @@
         </is>
       </c>
       <c r="C6" s="3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" s="3" t="n">
         <v>4</v>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
+          <t>sillas_vip</t>
+        </is>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>195000</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="n">
+        <v>89005408</v>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>Ruben</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" s="3" t="inlineStr">
+        <is>
           <t>sillas_regular</t>
         </is>
       </c>
-      <c r="F6" s="3" t="n">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="4" t="inlineStr">
+      <c r="F7" s="3" t="n">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="inlineStr">
         <is>
           <t>Tipo de Silla</t>
         </is>
       </c>
-      <c r="B9" s="4" t="inlineStr">
+      <c r="B10" s="4" t="inlineStr">
         <is>
           <t>Total Recaudado</t>
         </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>sillas_regular</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>100000</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>sillas_regular</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
           <t>sillas_vip</t>
         </is>
       </c>
-      <c r="B11" t="n">
-        <v>250000</v>
+      <c r="B12" t="n">
+        <v>585000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se implemento la manera de poder visualizar los boletos (Se creao al clase Boletos con su proxy, fxml y Db)
</commit_message>
<xml_diff>
--- a/proyecto_final_programacion_copia/src/main/java/co/edu/uniquindio/poo/Balance/Excel/Eventos_Personas.xlsx
+++ b/proyecto_final_programacion_copia/src/main/java/co/edu/uniquindio/poo/Balance/Excel/Eventos_Personas.xlsx
@@ -8,9 +8,7 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Kiss" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Colombia-Argentina" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Akash" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="One Direction" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Akash" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -287,120 +285,6 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:t>Ingresos Comparativos por Tipo de Silla - Colombia-Argentina</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <barChart>
-        <barDir val="col"/>
-        <grouping val="clustered"/>
-        <varyColors val="1"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <strRef>
-              <f>'Colombia-Argentina'!B9</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Colombia-Argentina'!$A$10:$A$11</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Colombia-Argentina'!$B$10:$B$11</f>
-            </numRef>
-          </val>
-        </ser>
-        <gapWidth val="150"/>
-        <axId val="10"/>
-        <axId val="100"/>
-      </barChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Tipo de Silla</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Ingresos Totales</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="10"/>
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
               <a:t>Ingresos Comparativos por Tipo de Silla - Akash</a:t>
             </a:r>
           </a:p>
@@ -417,7 +301,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Akash'!B9</f>
+              <f>'Akash'!B8</f>
             </strRef>
           </tx>
           <spPr>
@@ -427,126 +311,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Akash'!$A$10:$A$11</f>
+              <f>'Akash'!$A$9:$A$10</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Akash'!$B$10:$B$11</f>
-            </numRef>
-          </val>
-        </ser>
-        <gapWidth val="150"/>
-        <axId val="10"/>
-        <axId val="100"/>
-      </barChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Tipo de Silla</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Ingresos Totales</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="10"/>
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Ingresos Comparativos por Tipo de Silla - One Direction</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <barChart>
-        <barDir val="col"/>
-        <grouping val="clustered"/>
-        <varyColors val="1"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <strRef>
-              <f>'One Direction'!B10</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'One Direction'!$A$11:$A$12</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'One Direction'!$B$11:$B$12</f>
+              <f>'Akash'!$B$9:$B$10</f>
             </numRef>
           </val>
         </ser>
@@ -649,61 +419,7 @@
     <from>
       <col>4</col>
       <colOff>0</colOff>
-      <row>8</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="1" name="Chart 1"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>4</col>
-      <colOff>0</colOff>
-      <row>8</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="1" name="Chart 1"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>4</col>
-      <colOff>0</colOff>
-      <row>9</row>
+      <row>7</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="5400000" cy="2700000"/>
@@ -1075,7 +791,7 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>Manuel</t>
+          <t>Mauel</t>
         </is>
       </c>
       <c r="C4" s="3" t="n">
@@ -1086,20 +802,20 @@
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>sillas_vip</t>
+          <t>sillas_regular</t>
         </is>
       </c>
       <c r="F4" s="3" t="n">
-        <v>312500</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
-        <v>1094891731</v>
+        <v>65126523</v>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>Laura</t>
+          <t>Santiago</t>
         </is>
       </c>
       <c r="C5" s="3" t="n">
@@ -1114,31 +830,31 @@
         </is>
       </c>
       <c r="F5" s="3" t="n">
-        <v>312500</v>
+        <v>187500</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="n">
-        <v>1092455585</v>
+        <v>1094891731</v>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>Leonardo</t>
+          <t>Laura</t>
         </is>
       </c>
       <c r="C6" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>sillas_regular</t>
+          <t>sillas_vip</t>
         </is>
       </c>
       <c r="F6" s="3" t="n">
-        <v>250000</v>
+        <v>187500</v>
       </c>
     </row>
     <row r="9">
@@ -1160,7 +876,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>250000</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="11">
@@ -1170,7 +886,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>625000</v>
+        <v>375000</v>
       </c>
     </row>
   </sheetData>
@@ -1188,182 +904,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="41" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="10" customWidth="1" min="3" max="3"/>
-    <col width="9" customWidth="1" min="4" max="4"/>
-    <col width="16" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Detalles del Evento: Colombia-Argentina</t>
-        </is>
-      </c>
-    </row>
-    <row r="2"/>
-    <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>idPersona</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>nombrePersona</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>idEvento</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
-          <t>idSilla</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="inlineStr">
-        <is>
-          <t>tipoSilla</t>
-        </is>
-      </c>
-      <c r="F3" s="2" t="inlineStr">
-        <is>
-          <t>totalPagar</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="n">
-        <v>1094895528</v>
-      </c>
-      <c r="B4" s="3" t="inlineStr">
-        <is>
-          <t>Santiago</t>
-        </is>
-      </c>
-      <c r="C4" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D4" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="E4" s="3" t="inlineStr">
-        <is>
-          <t>sillas_vip</t>
-        </is>
-      </c>
-      <c r="F4" s="3" t="n">
-        <v>300000</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="n">
-        <v>89489489</v>
-      </c>
-      <c r="B5" s="3" t="inlineStr">
-        <is>
-          <t>Leonardo</t>
-        </is>
-      </c>
-      <c r="C5" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D5" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E5" s="3" t="inlineStr">
-        <is>
-          <t>sillas_vip</t>
-        </is>
-      </c>
-      <c r="F5" s="3" t="n">
-        <v>300000</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="n">
-        <v>1092455543</v>
-      </c>
-      <c r="B6" s="3" t="inlineStr">
-        <is>
-          <t>Manuel</t>
-        </is>
-      </c>
-      <c r="C6" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D6" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="E6" s="3" t="inlineStr">
-        <is>
-          <t>sillas_regular</t>
-        </is>
-      </c>
-      <c r="F6" s="3" t="n">
-        <v>200000</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="4" t="inlineStr">
-        <is>
-          <t>Tipo de Silla</t>
-        </is>
-      </c>
-      <c r="B9" s="4" t="inlineStr">
-        <is>
-          <t>Total Recaudado</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>sillas_regular</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>200000</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>sillas_vip</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>600000</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1375,7 +916,7 @@
     <col width="15" customWidth="1" min="2" max="2"/>
     <col width="10" customWidth="1" min="3" max="3"/>
     <col width="9" customWidth="1" min="4" max="4"/>
-    <col width="16" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
     <col width="12" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -1429,7 +970,7 @@
         </is>
       </c>
       <c r="C4" s="3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" s="3" t="n">
         <v>3</v>
@@ -1440,7 +981,7 @@
         </is>
       </c>
       <c r="F4" s="3" t="n">
-        <v>55000</v>
+        <v>75000</v>
       </c>
     </row>
     <row r="5">
@@ -1453,7 +994,7 @@
         </is>
       </c>
       <c r="C5" s="3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" s="3" t="n">
         <v>2</v>
@@ -1464,43 +1005,29 @@
         </is>
       </c>
       <c r="F5" s="3" t="n">
-        <v>55000</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="n">
-        <v>89005408</v>
-      </c>
-      <c r="B6" s="3" t="inlineStr">
-        <is>
-          <t>Ruben</t>
-        </is>
-      </c>
-      <c r="C6" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="D6" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="E6" s="3" t="inlineStr">
-        <is>
-          <t>sillas_regular</t>
-        </is>
-      </c>
-      <c r="F6" s="3" t="n">
-        <v>50000</v>
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="inlineStr">
+        <is>
+          <t>Tipo de Silla</t>
+        </is>
+      </c>
+      <c r="B8" s="4" t="inlineStr">
+        <is>
+          <t>Total Recaudado</t>
+        </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="inlineStr">
-        <is>
-          <t>Tipo de Silla</t>
-        </is>
-      </c>
-      <c r="B9" s="4" t="inlineStr">
-        <is>
-          <t>Total Recaudado</t>
-        </is>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>sillas_vip</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>150000</v>
       </c>
     </row>
     <row r="10">
@@ -1510,216 +1037,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>sillas_vip</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>110000</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="36" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="10" customWidth="1" min="3" max="3"/>
-    <col width="9" customWidth="1" min="4" max="4"/>
-    <col width="16" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Detalles del Evento: One Direction</t>
-        </is>
-      </c>
-    </row>
-    <row r="2"/>
-    <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>idPersona</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>nombrePersona</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>idEvento</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
-          <t>idSilla</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="inlineStr">
-        <is>
-          <t>tipoSilla</t>
-        </is>
-      </c>
-      <c r="F3" s="2" t="inlineStr">
-        <is>
-          <t>totalPagar</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="n">
-        <v>6526965</v>
-      </c>
-      <c r="B4" s="3" t="inlineStr">
-        <is>
-          <t>Carlos</t>
-        </is>
-      </c>
-      <c r="C4" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="D4" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="E4" s="3" t="inlineStr">
-        <is>
-          <t>sillas_vip</t>
-        </is>
-      </c>
-      <c r="F4" s="3" t="n">
-        <v>195000</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="n">
-        <v>6525695</v>
-      </c>
-      <c r="B5" s="3" t="inlineStr">
-        <is>
-          <t>valentina</t>
-        </is>
-      </c>
-      <c r="C5" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="D5" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E5" s="3" t="inlineStr">
-        <is>
-          <t>sillas_vip</t>
-        </is>
-      </c>
-      <c r="F5" s="3" t="n">
-        <v>195000</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="n">
-        <v>1092455543</v>
-      </c>
-      <c r="B6" s="3" t="inlineStr">
-        <is>
-          <t>Manuel</t>
-        </is>
-      </c>
-      <c r="C6" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="D6" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="E6" s="3" t="inlineStr">
-        <is>
-          <t>sillas_vip</t>
-        </is>
-      </c>
-      <c r="F6" s="3" t="n">
-        <v>195000</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="n">
-        <v>89005408</v>
-      </c>
-      <c r="B7" s="3" t="inlineStr">
-        <is>
-          <t>Ruben</t>
-        </is>
-      </c>
-      <c r="C7" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="D7" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E7" s="3" t="inlineStr">
-        <is>
-          <t>sillas_regular</t>
-        </is>
-      </c>
-      <c r="F7" s="3" t="n">
-        <v>150000</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="4" t="inlineStr">
-        <is>
-          <t>Tipo de Silla</t>
-        </is>
-      </c>
-      <c r="B10" s="4" t="inlineStr">
-        <is>
-          <t>Total Recaudado</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>sillas_regular</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>150000</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>sillas_vip</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>585000</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>